<commit_message>
*update documentation/ScrumProject.xlsx +added 17-May meeting folder
</commit_message>
<xml_diff>
--- a/documentation/ScrumProject.xlsx
+++ b/documentation/ScrumProject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Edu\PROG6001-Managing Software developement\Assignment3\PROG6001_Assignment\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A5B1D1-C731-40B9-ADE8-2361BA2F4F4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF1DEC7-B98B-426E-B4DC-0501C0E99A72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
   <si>
     <t>Sprint</t>
   </si>
@@ -128,6 +128,21 @@
   </si>
   <si>
     <t>Deadline</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Test file does not work, error code "No test executed"</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Completion date</t>
+  </si>
+  <si>
+    <t>Test case does not work</t>
   </si>
 </sst>
 </file>
@@ -482,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,9 +510,11 @@
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -513,8 +530,14 @@
       <c r="E1" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -530,8 +553,14 @@
       <c r="E2" s="6">
         <v>44334</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F2" s="6">
+        <v>44330</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -547,8 +576,14 @@
       <c r="E3" s="6">
         <v>44340</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F3" s="6">
+        <v>44331</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -564,8 +599,10 @@
       <c r="E4" s="6">
         <v>44344</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -581,8 +618,10 @@
       <c r="E5" s="6">
         <v>44348</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -598,6 +637,8 @@
       <c r="E6" s="6">
         <v>44351</v>
       </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -607,10 +648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498A3FAB-7D1B-4D46-9F76-203360044486}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,9 +660,10 @@
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,8 +676,11 @@
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -646,10 +691,11 @@
         <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -660,10 +706,11 @@
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -674,10 +721,11 @@
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -690,8 +738,11 @@
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -702,10 +753,11 @@
         <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -716,10 +768,11 @@
         <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -730,10 +783,11 @@
         <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -744,10 +798,13 @@
         <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -758,10 +815,11 @@
         <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -772,10 +830,11 @@
         <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>3</v>
       </c>
@@ -786,10 +845,11 @@
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>3</v>
       </c>
@@ -800,10 +860,11 @@
         <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>4</v>
       </c>
@@ -816,8 +877,9 @@
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>4</v>
       </c>
@@ -830,8 +892,9 @@
       <c r="D15" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>4</v>
       </c>
@@ -844,8 +907,9 @@
       <c r="D16" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>5</v>
       </c>
@@ -858,8 +922,9 @@
       <c r="D17" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>5</v>
       </c>
@@ -872,8 +937,9 @@
       <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>5</v>
       </c>
@@ -886,8 +952,9 @@
       <c r="D19" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>5</v>
       </c>
@@ -900,6 +967,7 @@
       <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="E20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* update documentation/ScrumProject.xlsx 4/6
</commit_message>
<xml_diff>
--- a/documentation/ScrumProject.xlsx
+++ b/documentation/ScrumProject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\Edu\PROG6001-Managing Software developement\Assignment3\PROG6001_Assignment\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD1DC3F-AA92-48EE-B320-17E91DFA309D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45B25BB-631A-43AE-9735-6595843FB732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>Sprint</t>
   </si>
@@ -34,30 +34,18 @@
     <t>Status</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Sprint name</t>
   </si>
   <si>
     <t>Sprint number</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
-    <t>Adding method comments/cleaning the code</t>
-  </si>
-  <si>
     <t>Add Attack action</t>
   </si>
   <si>
-    <t>Provide additional information to user regarding room/item</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -106,9 +94,6 @@
     <t>Add instructions, descriptions</t>
   </si>
   <si>
-    <t>Test desciptions</t>
-  </si>
-  <si>
     <t>Design documentation</t>
   </si>
   <si>
@@ -197,6 +182,12 @@
   </si>
   <si>
     <t>Accept</t>
+  </si>
+  <si>
+    <t>Adding method comments/cleaning the code/ generate Javadoc</t>
+  </si>
+  <si>
+    <t>Provide additional information to user regarding room/item/game</t>
   </si>
 </sst>
 </file>
@@ -261,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -280,6 +271,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,13 +555,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
@@ -582,54 +575,54 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -641,30 +634,30 @@
         <v>44330</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -676,30 +669,30 @@
         <v>44331</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3">
         <v>2</v>
@@ -716,19 +709,19 @@
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3">
         <v>3</v>
@@ -736,32 +729,34 @@
       <c r="G5" s="6">
         <v>44348</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="6">
+        <v>44348</v>
+      </c>
       <c r="I5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="K5" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F6" s="3">
         <v>3</v>
@@ -769,7 +764,9 @@
       <c r="G6" s="6">
         <v>44351</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="6">
+        <v>44351</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -784,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498A3FAB-7D1B-4D46-9F76-203360044486}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +791,7 @@
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64" customWidth="1"/>
+    <col min="5" max="5" width="57.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -802,16 +799,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -819,13 +816,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -834,13 +831,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -849,13 +846,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -864,16 +861,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -881,13 +878,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -896,13 +893,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -911,13 +908,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -926,16 +923,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -943,13 +940,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -958,13 +955,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -973,13 +970,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -988,13 +985,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -1003,13 +1000,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -1018,45 +1015,43 @@
         <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -1065,13 +1060,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -1080,30 +1075,24 @@
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>5</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="3"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>